<commit_message>
remove CLOSING PHASE & fix FE bugs
</commit_message>
<xml_diff>
--- a/docs/BDP305x_TestCases.xlsx
+++ b/docs/BDP305x_TestCases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Dapp\funix-pricing-chain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C6EEF-F36D-40FB-B970-3D431156CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="821" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="821" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Participant!$A$8:$I$15</definedName>
     <definedName name="ACTION">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,12 +67,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -297,12 +298,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>close session</t>
-  </si>
-  <si>
-    <t>close session change state to "CLOSING"</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -315,9 +310,6 @@
     <t>session is in "OPENED" state</t>
   </si>
   <si>
-    <t>session is in "CLOSING" state</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -325,9 +317,6 @@
   </si>
   <si>
     <t>get all users information</t>
-  </si>
-  <si>
-    <t>9</t>
   </si>
   <si>
     <t>update session detail</t>
@@ -414,31 +403,11 @@
     <t>Participant</t>
   </si>
   <si>
-    <t>Close session</t>
-  </si>
-  <si>
-    <t>change the state of the session to "CLOSING"</t>
-  </si>
-  <si>
     <t>1. Connect to Dapp with Metamask with Admin address
 2. Choose a session to change the information 
 3. Click "Update Session Detail" button and then fill in the name, description, images(if available) then confirm the transaction</t>
   </si>
   <si>
-    <t>1. Connect to Dapp with Metamask with Admin address
-2. Choose a session to close
-3. Click "Close" button then confirm the transaction</t>
-  </si>
-  <si>
-    <t>State of the session should change to CLOSING and "Set final price" is displayed</t>
-  </si>
-  <si>
-    <t>State is changed to "CLOSING" and "Set final price" section is displayed</t>
-  </si>
-  <si>
-    <t>Admin-5.1</t>
-  </si>
-  <si>
     <t>After closing session</t>
   </si>
   <si>
@@ -451,9 +420,6 @@
   </si>
   <si>
     <t>Final price of the session is stored and state of the session changes to "CLOSED" and deviation, # of joined sessions of participants who joined the session should be updated</t>
-  </si>
-  <si>
-    <t>Session must in "CLOSING" state</t>
   </si>
   <si>
     <t>State is changed to "CLOSED" and final price of the session is stored and deviation as well as # of joined sessions of participants who joined are updated</t>
@@ -563,7 +529,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
   </numFmts>
@@ -1054,90 +1020,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1153,8 +1109,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1210,23 +1165,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFill="1"/>
@@ -1237,30 +1186,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1291,19 +1238,19 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1336,7 +1283,7 @@
     <xf numFmtId="49" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1349,10 +1296,13 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1360,19 +1310,16 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2 23" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal_Functional Test Case v1.0" xfId="4"/>
-    <cellStyle name="Normal_Sheet1" xfId="5"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="6"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2 23" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal_Functional Test Case v1.0" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1734,479 +1681,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="1.875" style="69" customWidth="1"/>
-    <col min="2" max="8" width="8.25" style="69" customWidth="1"/>
-    <col min="9" max="10" width="14.375" style="69" customWidth="1"/>
-    <col min="11" max="13" width="8.25" style="69" customWidth="1"/>
-    <col min="14" max="14" width="8.625" style="69" customWidth="1"/>
-    <col min="15" max="15" width="7.25" style="69" customWidth="1"/>
-    <col min="16" max="16" width="4.375" style="69" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="69"/>
+    <col min="1" max="1" width="1.88671875" style="60" customWidth="1"/>
+    <col min="2" max="8" width="8.21875" style="60" customWidth="1"/>
+    <col min="9" max="10" width="14.33203125" style="60" customWidth="1"/>
+    <col min="11" max="13" width="8.21875" style="60" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="60" customWidth="1"/>
+    <col min="15" max="15" width="7.21875" style="60" customWidth="1"/>
+    <col min="16" max="16" width="4.33203125" style="60" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="60"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="73"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="64"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="77"/>
-    </row>
-    <row r="4" spans="2:15" ht="18.75">
-      <c r="B4" s="74"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="77"/>
-    </row>
-    <row r="5" spans="2:15" ht="18.75">
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="77"/>
+      <c r="B3" s="65"/>
+      <c r="D3" s="66"/>
+      <c r="O3" s="67"/>
+    </row>
+    <row r="4" spans="2:15" ht="18">
+      <c r="B4" s="65"/>
+      <c r="D4" s="68"/>
+      <c r="O4" s="67"/>
+    </row>
+    <row r="5" spans="2:15" ht="18">
+      <c r="B5" s="65"/>
+      <c r="D5" s="68"/>
+      <c r="O5" s="67"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="74"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="77"/>
+      <c r="B6" s="65"/>
+      <c r="O6" s="67"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="74"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
-      <c r="O7" s="77"/>
+      <c r="B7" s="65"/>
+      <c r="D7" s="69"/>
+      <c r="O7" s="67"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="74"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="77"/>
-    </row>
-    <row r="9" spans="2:15" ht="23.25">
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="77"/>
-    </row>
-    <row r="10" spans="2:15" ht="38.65" customHeight="1">
-      <c r="B10" s="100" t="s">
+      <c r="B8" s="65"/>
+      <c r="D8" s="69"/>
+      <c r="O8" s="67"/>
+    </row>
+    <row r="9" spans="2:15" ht="22.8">
+      <c r="B9" s="65"/>
+      <c r="E9" s="70"/>
+      <c r="O9" s="67"/>
+    </row>
+    <row r="10" spans="2:15" ht="38.700000000000003" customHeight="1">
+      <c r="B10" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="102"/>
-    </row>
-    <row r="11" spans="2:15" ht="37.15" customHeight="1">
-      <c r="B11" s="100" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="91"/>
+    </row>
+    <row r="11" spans="2:15" ht="37.200000000000003" customHeight="1">
+      <c r="B11" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="102"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="91"/>
     </row>
     <row r="12" spans="2:15" ht="30">
-      <c r="B12" s="96"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="98"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="87"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="77"/>
+      <c r="B13" s="65"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="74"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="77"/>
+      <c r="B14" s="65"/>
+      <c r="O14" s="67"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="74"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="103" t="s">
+      <c r="B15" s="65"/>
+      <c r="F15" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="105" t="s">
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="105"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="77"/>
+      <c r="J15" s="94"/>
+      <c r="O15" s="67"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="74"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="106" t="s">
+      <c r="B16" s="65"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="77"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="O16" s="67"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="74"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="77"/>
+      <c r="B17" s="65"/>
+      <c r="O17" s="67"/>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="74"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="77"/>
+      <c r="B18" s="65"/>
+      <c r="O18" s="67"/>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="77"/>
+      <c r="B19" s="65"/>
+      <c r="O19" s="67"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="74"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="77"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="O20" s="67"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="74"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="77"/>
+      <c r="B21" s="65"/>
+      <c r="O21" s="67"/>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="74"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="77"/>
+      <c r="B22" s="65"/>
+      <c r="O22" s="67"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="74"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="99"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="77"/>
+      <c r="B23" s="65"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="O23" s="67"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
-      <c r="N24" s="84"/>
-      <c r="O24" s="85"/>
-    </row>
-    <row r="25" spans="2:15">
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
-    </row>
-    <row r="26" spans="2:15">
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-    </row>
-    <row r="27" spans="2:15">
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-    </row>
-    <row r="28" spans="2:15">
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-    </row>
-    <row r="29" spans="2:15">
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="75"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-    </row>
-    <row r="31" spans="2:15">
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2230,270 +1919,253 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="1.375" style="37" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="37" customWidth="1"/>
-    <col min="3" max="3" width="23.75" style="39" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="39" customWidth="1"/>
-    <col min="5" max="5" width="49.625" style="39" customWidth="1"/>
-    <col min="6" max="6" width="30.625" style="39" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="37"/>
+    <col min="1" max="1" width="1.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="33" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:6" ht="24.6">
+      <c r="A1" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
-      <c r="B2" s="38"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="32"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-    </row>
-    <row r="4" spans="1:6" s="41" customFormat="1" ht="84.75" customHeight="1">
-      <c r="B4" s="110" t="s">
+      <c r="C3" s="101"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+    </row>
+    <row r="4" spans="1:6" s="35" customFormat="1" ht="84.75" customHeight="1">
+      <c r="B4" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-    </row>
-    <row r="6" spans="1:6" s="44" customFormat="1">
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-    </row>
-    <row r="7" spans="1:6" s="47" customFormat="1" ht="21" customHeight="1">
-      <c r="B7" s="48" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" s="37" customFormat="1">
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:6" s="40" customFormat="1" ht="21" customHeight="1">
+      <c r="B7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="52">
+      <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="52">
+      <c r="B9" s="45">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" s="52">
+      <c r="B10" s="45">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="52">
+      <c r="B11" s="45">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="52">
+      <c r="B12" s="45">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="52"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="52"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="52"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="53"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2514,468 +2186,427 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="11.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="20"/>
-    <col min="9" max="9" width="17.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.25" style="21" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="16.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="16" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+    <row r="1" spans="1:11" s="5" customFormat="1">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="92" t="s">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A3" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="115" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="8"/>
+      <c r="K3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="11" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="92" t="s">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="116" t="s">
+      <c r="E5" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="11" t="s">
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="54">
-        <f>COUNTIF(G10:G995,"Pass")</f>
-        <v>7</v>
-      </c>
-      <c r="B6" s="54">
-        <f>COUNTIF(G10:G995,"Fail")</f>
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="47">
+        <f>COUNTIF(G10:G993,"Pass")</f>
+        <v>6</v>
+      </c>
+      <c r="B6" s="47">
+        <f>COUNTIF(G10:G993,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="47">
         <f>E6-D6-B6-A6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="54">
-        <f>COUNTIF(G$10:G$995,"N/A")</f>
+      <c r="D6" s="47">
+        <f>COUNTIF(G$10:G$993,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="114">
-        <f>COUNTA(A10:A995)</f>
-        <v>7</v>
-      </c>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A8" s="55" t="s">
+      <c r="E6" s="103">
+        <f>COUNTA(A10:A993)</f>
+        <v>6</v>
+      </c>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="G8" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="95"/>
-      <c r="B9" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" s="19" customFormat="1" ht="121.15" customHeight="1">
-      <c r="A10" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="56" t="s">
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="84"/>
+      <c r="B9" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:11" s="15" customFormat="1" ht="121.2" customHeight="1">
+      <c r="A10" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="F10" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="56" t="s">
+      <c r="C10" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="83">
+        <v>44810</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="84"/>
+      <c r="B11" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:11" ht="79.2">
+      <c r="A12" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="83">
+        <v>44810</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="84"/>
+      <c r="B13" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" ht="26.4">
+      <c r="A14" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="94">
+      <c r="E14" s="49"/>
+      <c r="F14" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="83">
         <v>44810</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="95"/>
-      <c r="B11" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" ht="76.5">
-      <c r="A12" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="56" t="s">
+      <c r="I14" s="50"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="84"/>
+      <c r="B15" s="84" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" ht="66">
+      <c r="A16" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="94">
+      <c r="H16" s="83">
         <v>44810</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="95"/>
-      <c r="B13" s="95" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" ht="25.5">
-      <c r="A14" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="94">
+      <c r="I16" s="50"/>
+    </row>
+    <row r="17" spans="1:9" ht="26.4">
+      <c r="A17" s="84"/>
+      <c r="B17" s="84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+    </row>
+    <row r="18" spans="1:9" ht="132">
+      <c r="A18" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="83">
         <v>44810</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="95"/>
-      <c r="B15" s="95" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" ht="63.75">
-      <c r="A16" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" s="94">
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="1:9" ht="26.4">
+      <c r="A19" s="84"/>
+      <c r="B19" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+    </row>
+    <row r="20" spans="1:9" ht="118.8">
+      <c r="A20" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="83">
         <v>44810</v>
       </c>
-      <c r="I16" s="57"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="95"/>
-      <c r="B17" s="95" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-    </row>
-    <row r="18" spans="1:9" ht="102">
-      <c r="A18" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="94">
-        <v>44810</v>
-      </c>
-      <c r="I18" s="57"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="95"/>
-      <c r="B19" s="95" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-    </row>
-    <row r="20" spans="1:9" ht="63.75">
-      <c r="A20" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="94">
-        <v>44810</v>
-      </c>
-      <c r="I20" s="57"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="95"/>
-      <c r="B21" s="95" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-    </row>
-    <row r="22" spans="1:9" ht="102">
-      <c r="A22" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="56" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="94">
-        <v>44810</v>
-      </c>
-      <c r="I22" s="57"/>
+      <c r="I20" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2987,11 +2618,11 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7:G9 G1:G4 G23:G142">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7:G9 G1:G4 G21:G140" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$K$2:$K$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G10:G22">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G10:G20" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$K$2:$K$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -3006,377 +2637,373 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="20"/>
-    <col min="9" max="9" width="17.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="16.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+    <row r="1" spans="1:11">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="92" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1">
+      <c r="A2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="20" customFormat="1" ht="25.5">
-      <c r="A3" s="92" t="s">
+    <row r="3" spans="1:11" ht="26.4">
+      <c r="A3" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="121" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="106" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="92" t="s">
+    <row r="4" spans="1:11" ht="18" customHeight="1">
+      <c r="A4" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="20" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A5" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="116" t="s">
+      <c r="E5" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="20" t="s">
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="54">
+    <row r="6" spans="1:11" ht="15" customHeight="1">
+      <c r="A6" s="47">
         <f>COUNTIF(G10:G998,"Pass")</f>
         <v>4</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="47">
         <f>COUNTIF(G10:G998,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="47">
         <f>E6-D6-B6-A6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="47">
         <f>COUNTIF(G$10:G$998,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="114">
+      <c r="E6" s="103">
         <f>COUNTA(A10:A998)</f>
         <v>4</v>
       </c>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:12" s="20" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" ht="25.5" customHeight="1">
+      <c r="A8" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="G8" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="87"/>
-      <c r="B9" s="87" t="s">
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A9" s="76"/>
+      <c r="B9" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" s="25" customFormat="1" ht="121.15" customHeight="1">
-      <c r="A10" s="56" t="s">
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" s="20" customFormat="1" ht="121.2" customHeight="1">
+      <c r="A10" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="83">
+        <v>44810</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="76"/>
+      <c r="B11" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" ht="105.6">
+      <c r="A12" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="83">
+        <v>44810</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A13" s="76"/>
+      <c r="B13" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:11" ht="39.6">
+      <c r="A14" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="B14" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="C14" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="D14" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="94">
+      <c r="E14" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="83">
         <v>44810</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="87"/>
-      <c r="B11" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="24"/>
-    </row>
-    <row r="12" spans="1:12" ht="102">
-      <c r="A12" s="56" t="s">
+      <c r="I14" s="50"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="76"/>
+      <c r="B15" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+    </row>
+    <row r="16" spans="1:11" ht="79.2">
+      <c r="A16" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="94">
+      <c r="F16" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="83">
         <v>44810</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="24"/>
-    </row>
-    <row r="13" spans="1:12" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="1:12" ht="38.25">
-      <c r="A14" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="F14" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="94">
-        <v>44810</v>
-      </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="24"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="87"/>
-      <c r="B15" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" ht="76.5">
-      <c r="A16" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" s="94">
-        <v>44810</v>
-      </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="87"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="24"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="56"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3388,11 +3015,11 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G9 G19:G144">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G4 G7:G9 G19:G144" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$K$2:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G10:G18">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G10:G18" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>$K$2:$K$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3407,268 +3034,239 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
     <col min="4" max="7" width="9" style="1"/>
-    <col min="8" max="9" width="33.125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="33.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="12" customHeight="1">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="120" t="s">
+      <c r="D3" s="109"/>
+      <c r="E3" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="120"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54"/>
     </row>
     <row r="4" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="89" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="56" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="26"/>
-      <c r="B9" s="64">
+      <c r="B9" s="57">
         <v>1</v>
       </c>
-      <c r="C9" s="65" t="str">
+      <c r="C9" s="58" t="str">
         <f>Admin!B2</f>
         <v>Admin Functions</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="57">
         <f>Admin!A6</f>
-        <v>7</v>
-      </c>
-      <c r="E9" s="64">
+        <v>6</v>
+      </c>
+      <c r="E9" s="57">
         <f>Admin!B6</f>
         <v>0</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="57">
         <f>Admin!C6</f>
         <v>0</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="57">
         <f>Admin!D6</f>
         <v>0</v>
       </c>
-      <c r="H9" s="64">
+      <c r="H9" s="57">
         <f>Admin!E6</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="26"/>
-      <c r="B10" s="64">
+      <c r="B10" s="57">
         <v>2</v>
       </c>
-      <c r="C10" s="65" t="str">
+      <c r="C10" s="58" t="str">
         <f>Participant!B2</f>
         <v>Participant Functions</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="57">
         <f>Participant!A6</f>
         <v>4</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="57">
         <f>Participant!B6</f>
         <v>0</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="57">
         <f>Participant!C6</f>
         <v>0</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="57">
         <f>Participant!D6</f>
         <v>0</v>
       </c>
-      <c r="H10" s="64">
+      <c r="H10" s="57">
         <f>Participant!E6</f>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="26"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="26"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="68" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="59">
         <f>SUM(D7:D11)</f>
-        <v>11</v>
-      </c>
-      <c r="E12" s="67">
+        <v>10</v>
+      </c>
+      <c r="E12" s="59">
         <f>SUM(E7:E11)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="67">
+      <c r="F12" s="59">
         <f>SUM(F7:F11)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="67">
+      <c r="G12" s="59">
         <f>SUM(G7:G11)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="67">
+      <c r="H12" s="59">
         <f>SUM(H7:H11)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="26"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="B13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="36">
+      <c r="E14" s="30">
         <f>(D12+E12)*100/(H12-G12)</f>
         <v>100</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="36">
+      <c r="E15" s="30">
         <f>D12*100/(H12-G12)</f>
         <v>100</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="H15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>